<commit_message>
Made changes in item bank excel
</commit_message>
<xml_diff>
--- a/Item bank from DigiArvi 2025 - Final.xlsx
+++ b/Item bank from DigiArvi 2025 - Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdaadh\Desktop\Item bank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA0F6B4-5860-4AAF-B91E-DEEB1E692E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA71056-17FA-4F1F-9CDB-8F2FECA4845E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6548F41-5644-4F5F-8D9E-38C4DDB10409}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2509" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="993">
   <si>
     <t>label</t>
   </si>
@@ -3472,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D8EB27-DBD6-457E-8C41-DC95B8D34093}">
   <dimension ref="A1:BL467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="AG13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR35" sqref="AR35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6304,8 +6304,8 @@
       <c r="AM25" s="3"/>
       <c r="AN25" s="3"/>
       <c r="AO25" s="3"/>
-      <c r="AP25" s="4">
-        <v>3.4</v>
+      <c r="AP25" s="4" t="s">
+        <v>949</v>
       </c>
       <c r="AQ25" s="4"/>
       <c r="AR25" s="4"/>
@@ -6414,8 +6414,8 @@
       <c r="AM26" s="3"/>
       <c r="AN26" s="3"/>
       <c r="AO26" s="3"/>
-      <c r="AP26" s="4">
-        <v>3.4</v>
+      <c r="AP26" s="4" t="s">
+        <v>949</v>
       </c>
       <c r="AQ26" s="4"/>
       <c r="AR26" s="4"/>
@@ -6524,8 +6524,8 @@
       <c r="AM27" s="3"/>
       <c r="AN27" s="3"/>
       <c r="AO27" s="3"/>
-      <c r="AP27" s="4">
-        <v>3.4</v>
+      <c r="AP27" s="4" t="s">
+        <v>949</v>
       </c>
       <c r="AQ27" s="4"/>
       <c r="AR27" s="4"/>

</xml_diff>

<commit_message>
added table short changes
</commit_message>
<xml_diff>
--- a/Item bank from DigiArvi 2025 - Final.xlsx
+++ b/Item bank from DigiArvi 2025 - Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdaadh\Desktop\Item bank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA71056-17FA-4F1F-9CDB-8F2FECA4845E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E169A76-55A5-4CE2-BA6C-364E66A08E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6548F41-5644-4F5F-8D9E-38C4DDB10409}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="992">
   <si>
     <t>label</t>
   </si>
@@ -2913,9 +2913,6 @@
   </si>
   <si>
     <t>order</t>
-  </si>
-  <si>
-    <t>1 , 2</t>
   </si>
   <si>
     <t>S1: Thinking Skills (including Computational Thinking)</t>
@@ -3472,8 +3469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D8EB27-DBD6-457E-8C41-DC95B8D34093}">
   <dimension ref="A1:BL467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR35" sqref="AR35"/>
+    <sheetView tabSelected="1" topLeftCell="AG137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP162" sqref="AP162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3692,7 +3689,7 @@
     </row>
     <row r="3" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3701,7 +3698,7 @@
         <v>923</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1</v>
@@ -3713,55 +3710,55 @@
         <v>3</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>955</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>956</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>957</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>958</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>959</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>992</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>960</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>961</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>962</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>963</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>964</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>965</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>966</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>967</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>969</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>970</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>971</v>
       </c>
       <c r="Y3" s="4" t="s">
         <v>4</v>
@@ -3830,58 +3827,58 @@
         <v>946</v>
       </c>
       <c r="AU3" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="AV3" s="3" t="s">
         <v>974</v>
       </c>
-      <c r="AV3" s="3" t="s">
+      <c r="AW3" s="3" t="s">
         <v>975</v>
       </c>
-      <c r="AW3" s="3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>976</v>
       </c>
-      <c r="AX3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="AY3" s="3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>978</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
         <v>980</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>981</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BD3" s="3" t="s">
         <v>982</v>
       </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BE3" s="3" t="s">
         <v>983</v>
       </c>
-      <c r="BE3" s="3" t="s">
+      <c r="BF3" s="3" t="s">
         <v>984</v>
       </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BG3" s="3" t="s">
         <v>985</v>
       </c>
-      <c r="BG3" s="3" t="s">
+      <c r="BH3" s="4" t="s">
         <v>986</v>
       </c>
-      <c r="BH3" s="4" t="s">
+      <c r="BI3" s="4" t="s">
         <v>987</v>
       </c>
-      <c r="BI3" s="4" t="s">
+      <c r="BJ3" s="4" t="s">
         <v>988</v>
       </c>
-      <c r="BJ3" s="4" t="s">
+      <c r="BK3" s="4" t="s">
         <v>989</v>
       </c>
-      <c r="BK3" s="4" t="s">
+      <c r="BL3" s="4" t="s">
         <v>990</v>
-      </c>
-      <c r="BL3" s="4" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.35">
@@ -12250,7 +12247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>77</v>
       </c>
@@ -12486,7 +12483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>79</v>
       </c>
@@ -14092,7 +14089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>93</v>
       </c>
@@ -14540,7 +14537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>97</v>
       </c>
@@ -15684,7 +15681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>107</v>
       </c>
@@ -21255,7 +21252,7 @@
       <c r="AN158" s="3"/>
       <c r="AO158" s="3"/>
       <c r="AP158" s="4" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="AQ158" s="4">
         <v>1</v>
@@ -21365,7 +21362,7 @@
       <c r="AN159" s="3"/>
       <c r="AO159" s="3"/>
       <c r="AP159" s="4" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="AQ159" s="4">
         <v>1</v>

</xml_diff>